<commit_message>
Updated gene sequence ground truth sources
</commit_message>
<xml_diff>
--- a/tests/test_dna/ground_truth_components/sources.xlsx
+++ b/tests/test_dna/ground_truth_components/sources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/009cdea6a32dcdf3/Documentos/MSc_AI/Term_2/SE_Group_Project/Project/genomic_data_extraction/dna/test/ground_truth_components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/009cdea6a32dcdf3/Documentos/MSc_AI/Term_2/SE_Group_Project/Project/genomic_data_extraction/tests/test_dna/ground_truth_components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{1CA02B19-63E6-4CCE-A1A4-FCAD9F51D763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF0A6AD1-4242-4178-9830-9AE666C86FFE}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{1CA02B19-63E6-4CCE-A1A4-FCAD9F51D763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39FA8682-DA65-4D38-8ACE-715ABB237A4A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B6C4DF9B-E63B-42C0-BFBC-74B78D721398}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Sources</t>
   </si>
   <si>
-    <t>Homo sapiens</t>
-  </si>
-  <si>
     <t>hg38 ENST00000373020.9 (ucsc.edu)</t>
   </si>
   <si>
@@ -66,6 +63,27 @@
   </si>
   <si>
     <t>Transcript: EME29333 - Exons - Galdieria_sulphuraria - Ensembl Genomes 58</t>
+  </si>
+  <si>
+    <t>Gene: Cre01.g000017 (CHLRE_01g000017v5) - Marked-up sequence - Chlamydomonas_reinhardtii - Ensembl Genomes 58</t>
+  </si>
+  <si>
+    <t>Gene: Cre01.g000033 (CHLRE_01g000033v5) - Marked-up sequence - Chlamydomonas_reinhardtii - Ensembl Genomes 58</t>
+  </si>
+  <si>
+    <t>Cyanidioschyzon Merolae</t>
+  </si>
+  <si>
+    <t>Chlamydomonas Reinhardtii</t>
+  </si>
+  <si>
+    <t>Homo Sapiens</t>
+  </si>
+  <si>
+    <t>Gene: CMA001C - Marked-up sequence - Cyanidioschyzon_merolae - Ensembl Genomes 58</t>
+  </si>
+  <si>
+    <t>Gene: CMA004C - Marked-up sequence - Cyanidioschyzon_merolae - Ensembl Genomes 58</t>
   </si>
 </sst>
 </file>
@@ -150,9 +168,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +208,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -296,7 +314,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -438,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,11 +464,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5754397-F8DA-45EE-8F61-CAC94F746419}">
-  <dimension ref="B2:H5"/>
+  <dimension ref="B2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -470,35 +486,57 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
-        <v>8</v>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -508,6 +546,10 @@
     <hyperlink ref="D4" r:id="rId3" display="https://www.genome.jp/entry/sce:YDL059C" xr:uid="{EA0E21F6-9949-4257-8700-1EE3D86A98D2}"/>
     <hyperlink ref="C5" r:id="rId4" display="https://plants.ensembl.org/Galdieria_sulphuraria/Transcript/Exons?db=core;g=Gasu_33370;r=scaf_26:161786-162930;t=EME29332" xr:uid="{8327D7BB-B540-4ABC-B409-F2DAAC01FE7A}"/>
     <hyperlink ref="D5" r:id="rId5" display="https://plants.ensembl.org/Galdieria_sulphuraria/Transcript/Exons?db=core;g=Gasu_33380;r=scaf_26:162936-163760;t=EME29333" xr:uid="{0565C225-4543-40B8-BD3F-2C08A39682D6}"/>
+    <hyperlink ref="C6" r:id="rId6" display="https://plants.ensembl.org/Chlamydomonas_reinhardtii/Gene/Sequence?db=core;g=CHLRE_01g000017v5;r=1:18766-20237;t=PNW87736" xr:uid="{D8003FF4-290D-4D52-9116-AEEA8B269D32}"/>
+    <hyperlink ref="D6" r:id="rId7" display="https://plants.ensembl.org/Chlamydomonas_reinhardtii/Gene/Sequence?db=core;g=CHLRE_01g000033v5;r=1:20356-23957;t=PNW87737" xr:uid="{DF7F84B2-C071-4B65-949C-C11E38AB12DB}"/>
+    <hyperlink ref="C7" r:id="rId8" display="https://plants.ensembl.org/Cyanidioschyzon_merolae/Gene/Sequence?db=core;g=CMA001C;r=1:3374-6125;t=CMA001CT" xr:uid="{E08DC4DA-843B-446C-9009-5B398B80D117}"/>
+    <hyperlink ref="D7" r:id="rId9" display="https://plants.ensembl.org/Cyanidioschyzon_merolae/Gene/Sequence?db=core;g=CMA004C;r=1:13612-13980;t=CMA004CT" xr:uid="{9FD9772B-1675-442E-A97D-702EC5906D72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>